<commit_message>
Added files post Cut from v5 iter0
</commit_message>
<xml_diff>
--- a/v0-challengeTrial/iter0/Samples.xlsx
+++ b/v0-challengeTrial/iter0/Samples.xlsx
@@ -359,7 +359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH11"/>
+  <dimension ref="A1:AH33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,103 +544,103 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>4.099421069712029</v>
+        <v>3.397080863175625</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8955297877174047</v>
+        <v>0.9240008656720505</v>
       </c>
       <c r="D2" t="n">
-        <v>1.328538130469363</v>
+        <v>0.3701065235141885</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5879931721496041</v>
+        <v>-0.2522194300844778</v>
       </c>
       <c r="F2" t="n">
-        <v>0.008403550964778362</v>
+        <v>2.440669415729952</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5271460212194461</v>
+        <v>0.08600347289998123</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1572883827400285</v>
+        <v>1.789111401775034</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.02859124085790832</v>
+        <v>0.3907658641499288</v>
       </c>
       <c r="J2" t="n">
-        <v>0.327210835345849</v>
+        <v>1.880554492476189</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3445907073859744</v>
+        <v>-0.7476612229047855</v>
       </c>
       <c r="L2" t="n">
-        <v>2.544212794088919</v>
+        <v>2.010754590339833</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.8755631973163017</v>
+        <v>-0.03744596509399301</v>
       </c>
       <c r="N2" t="n">
-        <v>20.43746960204623</v>
+        <v>7.261717170513003</v>
       </c>
       <c r="O2" t="n">
-        <v>0.4997024886078958</v>
+        <v>0.6962589358505534</v>
       </c>
       <c r="P2" t="n">
-        <v>49.17725534414893</v>
+        <v>47.55566861372083</v>
       </c>
       <c r="Q2" t="n">
-        <v>50.76037871062222</v>
+        <v>35.92830953968374</v>
       </c>
       <c r="R2" t="n">
-        <v>14.78269794110216</v>
+        <v>15.49646748718814</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9243110262981498</v>
+        <v>1.618164515124167</v>
       </c>
       <c r="T2" t="n">
-        <v>3.041891906668114</v>
+        <v>3.175670275772172</v>
       </c>
       <c r="U2" t="n">
-        <v>28.85138532549574</v>
+        <v>41.0418815203324</v>
       </c>
       <c r="V2" t="n">
-        <v>8.636593804162688</v>
+        <v>8.260176564855193</v>
       </c>
       <c r="W2" t="n">
-        <v>11.48216514014198</v>
+        <v>88.49566042806742</v>
       </c>
       <c r="X2" t="n">
-        <v>69.19020492220217</v>
+        <v>51.26270404578221</v>
       </c>
       <c r="Y2" t="n">
-        <v>82.32530602468428</v>
+        <v>31.11910122782373</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.1129789784629358</v>
+        <v>0.04453845306801647</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.1427903162489189</v>
+        <v>0.01319605029269084</v>
       </c>
       <c r="AB2" t="n">
-        <v>6424.780437152316</v>
+        <v>8970.801641319933</v>
       </c>
       <c r="AC2" t="n">
-        <v>66316.46776020192</v>
+        <v>52425.33156379277</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.463626347982775</v>
+        <v>0.2933828406826772</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.8452127582962495</v>
+        <v>0.8752277239080073</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.8429736092238603</v>
+        <v>0.1917358527939789</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.1645564663118387</v>
+        <v>0.2951975932114798</v>
       </c>
       <c r="AH2" t="n">
-        <v>3.61784447255285</v>
+        <v>24.62978841093248</v>
       </c>
     </row>
     <row r="3">
@@ -648,103 +648,103 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2.262997243281908</v>
+        <v>4.577630988920094</v>
       </c>
       <c r="C3" t="n">
-        <v>0.490686580491322</v>
+        <v>0.4019773537716597</v>
       </c>
       <c r="D3" t="n">
-        <v>2.270864722230185</v>
+        <v>2.59496399648864</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1514090659624481</v>
+        <v>0.8801549196758669</v>
       </c>
       <c r="F3" t="n">
-        <v>1.004315609044483</v>
+        <v>0.3623565394018773</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3823143213067715</v>
+        <v>-0.09364776838163469</v>
       </c>
       <c r="H3" t="n">
-        <v>1.184144994554184</v>
+        <v>0.7868723394527044</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.5115268045902334</v>
+        <v>0.6122427281354357</v>
       </c>
       <c r="J3" t="n">
-        <v>2.32272680332345</v>
+        <v>2.688957662829238</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.9298534207025856</v>
+        <v>0.01121697413158085</v>
       </c>
       <c r="L3" t="n">
-        <v>1.143115348127254</v>
+        <v>2.811291632972974</v>
       </c>
       <c r="M3" t="n">
-        <v>-0.2037205019126878</v>
+        <v>-0.5025157408977881</v>
       </c>
       <c r="N3" t="n">
-        <v>9.101847396907694</v>
+        <v>28.50753513270875</v>
       </c>
       <c r="O3" t="n">
-        <v>1.60217305598543</v>
+        <v>0.5065506600127941</v>
       </c>
       <c r="P3" t="n">
-        <v>25.8309385360218</v>
+        <v>34.71545294139084</v>
       </c>
       <c r="Q3" t="n">
-        <v>70.03283890535151</v>
+        <v>49.5761621940006</v>
       </c>
       <c r="R3" t="n">
-        <v>18.66125789781022</v>
+        <v>7.216700180068916</v>
       </c>
       <c r="S3" t="n">
-        <v>0.3519088067885401</v>
+        <v>0.6613697747570284</v>
       </c>
       <c r="T3" t="n">
-        <v>7.036384352327564</v>
+        <v>5.297357655153063</v>
       </c>
       <c r="U3" t="n">
-        <v>167.3482047917488</v>
+        <v>50.0537107608237</v>
       </c>
       <c r="V3" t="n">
-        <v>1.359712942173407</v>
+        <v>1.527955407771908</v>
       </c>
       <c r="W3" t="n">
-        <v>7.514738034870584</v>
+        <v>93.67680502096663</v>
       </c>
       <c r="X3" t="n">
-        <v>72.0886964815801</v>
+        <v>99.41272232893404</v>
       </c>
       <c r="Y3" t="n">
-        <v>47.90317970755278</v>
+        <v>87.2471388511898</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.6662868671274742</v>
+        <v>0.09174281368765153</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.8739804215476251</v>
+        <v>0.6904032252558576</v>
       </c>
       <c r="AB3" t="n">
-        <v>7072.078101652684</v>
+        <v>5761.619991920139</v>
       </c>
       <c r="AC3" t="n">
-        <v>35343.22929743875</v>
+        <v>83061.75498616514</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.678547470509727</v>
+        <v>0.07751233852660694</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.5081492938434219</v>
+        <v>0.124300523442385</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.1469678539296895</v>
+        <v>0.8992528208299752</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.9014228033263896</v>
+        <v>0.2401840505819271</v>
       </c>
       <c r="AH3" t="n">
-        <v>66.03156030933773</v>
+        <v>54.96983504463792</v>
       </c>
     </row>
     <row r="4">
@@ -752,103 +752,103 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1.003578425059921</v>
+        <v>1.852091077571104</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2824499658498054</v>
+        <v>0.418780123413483</v>
       </c>
       <c r="D4" t="n">
-        <v>2.015626800112489</v>
+        <v>1.87920665267161</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9128432835202505</v>
+        <v>-0.1347969948701543</v>
       </c>
       <c r="F4" t="n">
-        <v>1.624450836893348</v>
+        <v>1.254148563007225</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.4954789509560893</v>
+        <v>-0.2182757252723297</v>
       </c>
       <c r="H4" t="n">
-        <v>2.914283499392474</v>
+        <v>1.518243850796262</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.3379098581067982</v>
+        <v>0.5208942719229108</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8979114895133944</v>
+        <v>1.706277923502698</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.6815633578629119</v>
+        <v>0.9373516292653024</v>
       </c>
       <c r="L4" t="n">
-        <v>2.329711335429307</v>
+        <v>0.4977194645286788</v>
       </c>
       <c r="M4" t="n">
-        <v>0.3545702832113542</v>
+        <v>-0.2648320580269491</v>
       </c>
       <c r="N4" t="n">
-        <v>24.92870134462933</v>
+        <v>18.00458088545615</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2340162692469465</v>
+        <v>0.6777726425378804</v>
       </c>
       <c r="P4" t="n">
-        <v>35.18680735648665</v>
+        <v>2.5781855312689</v>
       </c>
       <c r="Q4" t="n">
-        <v>83.37300117915615</v>
+        <v>94.07467448012474</v>
       </c>
       <c r="R4" t="n">
-        <v>9.12096612424738</v>
+        <v>18.10505473971267</v>
       </c>
       <c r="S4" t="n">
-        <v>0.5484859618190692</v>
+        <v>1.686348191151193</v>
       </c>
       <c r="T4" t="n">
-        <v>4.677667890890275</v>
+        <v>4.394517502618931</v>
       </c>
       <c r="U4" t="n">
-        <v>151.3015526337493</v>
+        <v>199.7249383255849</v>
       </c>
       <c r="V4" t="n">
-        <v>5.123298259173879</v>
+        <v>0.1716350958776421</v>
       </c>
       <c r="W4" t="n">
-        <v>33.11974804780056</v>
+        <v>47.3044452561818</v>
       </c>
       <c r="X4" t="n">
-        <v>36.37106087418503</v>
+        <v>42.34616683353492</v>
       </c>
       <c r="Y4" t="n">
-        <v>79.96024262582722</v>
+        <v>2.773359544926469</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.518699999331782</v>
+        <v>0.7540255054653557</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.6473027178885515</v>
+        <v>0.1429487200857992</v>
       </c>
       <c r="AB4" t="n">
-        <v>627.291559844879</v>
+        <v>5253.151979535424</v>
       </c>
       <c r="AC4" t="n">
-        <v>79202.72783373967</v>
+        <v>70586.8867838786</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.1452662996414887</v>
+        <v>0.6420308394518645</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.1090958213865251</v>
+        <v>0.8028106687899195</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.5286687590813912</v>
+        <v>0.03108736086500464</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.4144138871728727</v>
+        <v>0.00848626950834459</v>
       </c>
       <c r="AH4" t="n">
-        <v>95.36115056209891</v>
+        <v>74.36205480399813</v>
       </c>
     </row>
     <row r="5">
@@ -856,103 +856,103 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1.773791644535618</v>
+        <v>5.053748334836522</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3715918764545796</v>
+        <v>0.7682178407918653</v>
       </c>
       <c r="D5" t="n">
-        <v>1.784518096001391</v>
+        <v>0.9977201128593416</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7322371386635624</v>
+        <v>0.240351010335744</v>
       </c>
       <c r="F5" t="n">
-        <v>2.366849861831573</v>
+        <v>0.5545708466884651</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.1257607064750241</v>
+        <v>-0.7090674685646668</v>
       </c>
       <c r="H5" t="n">
-        <v>1.485091614283821</v>
+        <v>2.544748725900113</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.8617150528252213</v>
+        <v>-0.5268444441663116</v>
       </c>
       <c r="J5" t="n">
-        <v>1.445612781067292</v>
+        <v>1.28040022831686</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.1940545671708293</v>
+        <v>-0.9288366561240491</v>
       </c>
       <c r="L5" t="n">
-        <v>1.253156285133482</v>
+        <v>1.622590383001163</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9680196280319306</v>
+        <v>0.4306022409802768</v>
       </c>
       <c r="N5" t="n">
-        <v>6.299028140455223</v>
+        <v>5.773533988966987</v>
       </c>
       <c r="O5" t="n">
-        <v>1.27680690061855</v>
+        <v>1.590131814813998</v>
       </c>
       <c r="P5" t="n">
-        <v>7.346975982137027</v>
+        <v>46.83552872842307</v>
       </c>
       <c r="Q5" t="n">
-        <v>65.62417245789977</v>
+        <v>23.69797921822273</v>
       </c>
       <c r="R5" t="n">
-        <v>12.07201982553336</v>
+        <v>10.84000877629167</v>
       </c>
       <c r="S5" t="n">
-        <v>0.0523100228740006</v>
+        <v>0.5762074157720323</v>
       </c>
       <c r="T5" t="n">
-        <v>9.158849119771475</v>
+        <v>2.674422665762673</v>
       </c>
       <c r="U5" t="n">
-        <v>3.571763957793924</v>
+        <v>107.8387348905072</v>
       </c>
       <c r="V5" t="n">
-        <v>2.571674016925931</v>
+        <v>4.715682620057095</v>
       </c>
       <c r="W5" t="n">
-        <v>81.42619478455123</v>
+        <v>72.28479781989937</v>
       </c>
       <c r="X5" t="n">
-        <v>23.57630312265565</v>
+        <v>19.96076243733687</v>
       </c>
       <c r="Y5" t="n">
-        <v>5.639737981089834</v>
+        <v>71.30417722328943</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.8902857352740218</v>
+        <v>0.9350519970484076</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.3769299192048521</v>
+        <v>0.6142277303864513</v>
       </c>
       <c r="AB5" t="n">
-        <v>8409.57070315543</v>
+        <v>1617.408800760197</v>
       </c>
       <c r="AC5" t="n">
-        <v>56879.52973431452</v>
+        <v>49471.06519474283</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.7992422218364291</v>
+        <v>0.5919328504831309</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.4701743859391352</v>
+        <v>0.2895795245366833</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.07796875699759354</v>
+        <v>0.7789813060870149</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.533077262243974</v>
+        <v>0.5887903098044501</v>
       </c>
       <c r="AH5" t="n">
-        <v>18.81497856541939</v>
+        <v>39.84020944875695</v>
       </c>
     </row>
     <row r="6">
@@ -960,103 +960,103 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>5.93763132810894</v>
+        <v>5.620914908749544</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7697322277515203</v>
+        <v>0.5601330570258838</v>
       </c>
       <c r="D6" t="n">
-        <v>0.09804761995959747</v>
+        <v>1.615937259562898</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3896991344864561</v>
+        <v>-0.5392272965284578</v>
       </c>
       <c r="F6" t="n">
-        <v>1.334988663008528</v>
+        <v>2.234448740639944</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.6122517947581889</v>
+        <v>0.5128081002229252</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6864868959897781</v>
+        <v>0.3499168743654409</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3853453752775873</v>
+        <v>-0.8639199070454102</v>
       </c>
       <c r="J6" t="n">
-        <v>2.057360999162827</v>
+        <v>0.07807578100623978</v>
       </c>
       <c r="K6" t="n">
-        <v>0.580205042449685</v>
+        <v>-0.1402683854579013</v>
       </c>
       <c r="L6" t="n">
-        <v>2.071616396237106</v>
+        <v>0.3106290641107596</v>
       </c>
       <c r="M6" t="n">
-        <v>0.7741897010372265</v>
+        <v>-0.8221331940974459</v>
       </c>
       <c r="N6" t="n">
-        <v>15.39450646735811</v>
+        <v>20.7532741445399</v>
       </c>
       <c r="O6" t="n">
-        <v>0.9228463821450241</v>
+        <v>0.9448038938177635</v>
       </c>
       <c r="P6" t="n">
-        <v>41.2267088009212</v>
+        <v>31.02062659442408</v>
       </c>
       <c r="Q6" t="n">
-        <v>11.13530426384971</v>
+        <v>99.52784271486523</v>
       </c>
       <c r="R6" t="n">
-        <v>5.561381926245948</v>
+        <v>8.397251211782081</v>
       </c>
       <c r="S6" t="n">
-        <v>1.931962200034079</v>
+        <v>1.40274879427391</v>
       </c>
       <c r="T6" t="n">
-        <v>5.21016116363486</v>
+        <v>3.869882985652057</v>
       </c>
       <c r="U6" t="n">
-        <v>94.12317646906554</v>
+        <v>9.5697793369467</v>
       </c>
       <c r="V6" t="n">
-        <v>7.30264621571289</v>
+        <v>1.939641509545305</v>
       </c>
       <c r="W6" t="n">
-        <v>74.01118434113589</v>
+        <v>62.41912970169843</v>
       </c>
       <c r="X6" t="n">
-        <v>84.26474438514371</v>
+        <v>60.17945071423038</v>
       </c>
       <c r="Y6" t="n">
-        <v>12.25250496408835</v>
+        <v>72.94883193585765</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.3578724604885457</v>
+        <v>0.1651928473888282</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.7394086924860221</v>
+        <v>0.4463219882933867</v>
       </c>
       <c r="AB6" t="n">
-        <v>3635.760250126979</v>
+        <v>2515.679251406813</v>
       </c>
       <c r="AC6" t="n">
-        <v>19453.93733804055</v>
+        <v>45137.59448157773</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.2018684008796668</v>
+        <v>0.1386617332952407</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.6939625925761423</v>
+        <v>0.1539653830952664</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.6610853324042096</v>
+        <v>0.9368836336277636</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.2495652654652786</v>
+        <v>0.2656521580353352</v>
       </c>
       <c r="AH6" t="n">
-        <v>71.31139518017757</v>
+        <v>57.72213129254052</v>
       </c>
     </row>
     <row r="7">
@@ -1064,103 +1064,103 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1331430344475555</v>
+        <v>2.901887167291826</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9610462618265122</v>
+        <v>0.5157405818320919</v>
       </c>
       <c r="D7" t="n">
-        <v>1.166362353291737</v>
+        <v>1.565242142071194</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.6931565175010415</v>
+        <v>-0.7973620602940841</v>
       </c>
       <c r="F7" t="n">
-        <v>2.543525515991014</v>
+        <v>1.348646403143244</v>
       </c>
       <c r="G7" t="n">
-        <v>0.6709020934563885</v>
+        <v>-0.03399683257387065</v>
       </c>
       <c r="H7" t="n">
-        <v>2.541216459088877</v>
+        <v>2.760622612699806</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6322489028254017</v>
+        <v>0.8644091588108653</v>
       </c>
       <c r="J7" t="n">
-        <v>2.966795681370813</v>
+        <v>0.443549436552376</v>
       </c>
       <c r="K7" t="n">
-        <v>0.07054615648645157</v>
+        <v>0.6627384213287664</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1392101089423503</v>
+        <v>2.064510185406967</v>
       </c>
       <c r="M7" t="n">
-        <v>0.4336204679046918</v>
+        <v>0.3667149843485242</v>
       </c>
       <c r="N7" t="n">
-        <v>27.19043004877497</v>
+        <v>12.42596320925766</v>
       </c>
       <c r="O7" t="n">
-        <v>1.058249887891836</v>
+        <v>1.878144604212308</v>
       </c>
       <c r="P7" t="n">
-        <v>23.60097986801575</v>
+        <v>5.573774233139564</v>
       </c>
       <c r="Q7" t="n">
-        <v>3.799104585824018</v>
+        <v>29.07268862020742</v>
       </c>
       <c r="R7" t="n">
-        <v>0.5540630829413591</v>
+        <v>13.56307861170708</v>
       </c>
       <c r="S7" t="n">
-        <v>1.003105869185605</v>
+        <v>0.05186572402244791</v>
       </c>
       <c r="T7" t="n">
-        <v>0.8395528720910892</v>
+        <v>0.8465504386416877</v>
       </c>
       <c r="U7" t="n">
-        <v>124.349940434092</v>
+        <v>185.4184117405265</v>
       </c>
       <c r="V7" t="n">
-        <v>3.788918498884982</v>
+        <v>4.418852578517257</v>
       </c>
       <c r="W7" t="n">
-        <v>57.00780797317082</v>
+        <v>58.68522623922834</v>
       </c>
       <c r="X7" t="n">
-        <v>42.61761174466218</v>
+        <v>46.30317376634612</v>
       </c>
       <c r="Y7" t="n">
-        <v>52.79839252494827</v>
+        <v>15.24197657542377</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.4651261927969792</v>
+        <v>0.2050362171420863</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.5865085559195032</v>
+        <v>0.4969279840093141</v>
       </c>
       <c r="AB7" t="n">
-        <v>9052.554810077077</v>
+        <v>8568.129338693954</v>
       </c>
       <c r="AC7" t="n">
-        <v>42351.81528652897</v>
+        <v>26854.97970896904</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.8732405704304663</v>
+        <v>0.4083744685812336</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.04553357866606648</v>
+        <v>0.09069738934370966</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.7479245762870561</v>
+        <v>0.1326711919144909</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.8475492619966112</v>
+        <v>0.9881206963733991</v>
       </c>
       <c r="AH7" t="n">
-        <v>89.30749773121029</v>
+        <v>42.69858682685591</v>
       </c>
     </row>
     <row r="8">
@@ -1168,103 +1168,103 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>4.62656053880976</v>
+        <v>1.029568952588949</v>
       </c>
       <c r="C8" t="n">
-        <v>0.09161277734000089</v>
+        <v>0.0072165491551529</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5546672088665985</v>
+        <v>1.823573135805046</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3419778251957226</v>
+        <v>0.1464916746032743</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8271165801753375</v>
+        <v>2.691821539200018</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.2535528524989201</v>
+        <v>-0.9422625351247867</v>
       </c>
       <c r="H8" t="n">
-        <v>1.592418707128694</v>
+        <v>2.489388536287568</v>
       </c>
       <c r="I8" t="n">
-        <v>0.03390426190918361</v>
+        <v>-0.4135526335944466</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1787933778348564</v>
+        <v>0.1489876566681873</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6579780160750126</v>
+        <v>0.7946302336839823</v>
       </c>
       <c r="L8" t="n">
-        <v>2.945093222919822</v>
+        <v>1.540450354373726</v>
       </c>
       <c r="M8" t="n">
-        <v>-0.1261989001416388</v>
+        <v>0.7723877792908787</v>
       </c>
       <c r="N8" t="n">
-        <v>3.22356656805096</v>
+        <v>19.48187087767697</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1295195611424771</v>
+        <v>0.4065335510424721</v>
       </c>
       <c r="P8" t="n">
-        <v>17.3518853646575</v>
+        <v>10.67100146066229</v>
       </c>
       <c r="Q8" t="n">
-        <v>25.1342708319025</v>
+        <v>54.52423934593039</v>
       </c>
       <c r="R8" t="n">
-        <v>6.637270811527043</v>
+        <v>16.9580375200725</v>
       </c>
       <c r="S8" t="n">
-        <v>1.442043794530179</v>
+        <v>1.448236470349146</v>
       </c>
       <c r="T8" t="n">
-        <v>2.27802619399655</v>
+        <v>7.254192903822284</v>
       </c>
       <c r="U8" t="n">
-        <v>48.5724427916086</v>
+        <v>169.9802730518338</v>
       </c>
       <c r="V8" t="n">
-        <v>9.576236176389425</v>
+        <v>5.952912729409324</v>
       </c>
       <c r="W8" t="n">
-        <v>62.78129645817754</v>
+        <v>53.67871166771611</v>
       </c>
       <c r="X8" t="n">
-        <v>15.76998315306931</v>
+        <v>15.39208399400069</v>
       </c>
       <c r="Y8" t="n">
-        <v>91.60515599401722</v>
+        <v>5.447516531406238</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.2948653049086439</v>
+        <v>0.8549154676336154</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.993590711233182</v>
+        <v>0.8891956156227354</v>
       </c>
       <c r="AB8" t="n">
-        <v>1798.635175810697</v>
+        <v>8315.089344116568</v>
       </c>
       <c r="AC8" t="n">
-        <v>6126.237426029699</v>
+        <v>38198.6718623397</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.9382200297483807</v>
+        <v>0.4515614209774957</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.946749102729781</v>
+        <v>0.4914109561252112</v>
       </c>
       <c r="AF8" t="n">
-        <v>0.4808743688898677</v>
+        <v>0.9783428168481446</v>
       </c>
       <c r="AG8" t="n">
-        <v>0.002687022595864652</v>
+        <v>0.7912321214741775</v>
       </c>
       <c r="AH8" t="n">
-        <v>54.98426477829047</v>
+        <v>36.9275918448442</v>
       </c>
     </row>
     <row r="9">
@@ -1272,103 +1272,103 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>2.793414710612462</v>
+        <v>3.341386364134584</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5634897082853493</v>
+        <v>0.730461991002167</v>
       </c>
       <c r="D9" t="n">
-        <v>2.883882817659739</v>
+        <v>0.6555450812272812</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.169455375843918</v>
+        <v>0.9558992937068151</v>
       </c>
       <c r="F9" t="n">
-        <v>2.923902435994776</v>
+        <v>2.986646171331199</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.9774197396957777</v>
+        <v>0.9685163622391324</v>
       </c>
       <c r="H9" t="n">
-        <v>2.103515574700428</v>
+        <v>1.342946893064522</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4173091874220389</v>
+        <v>-0.9801053931789252</v>
       </c>
       <c r="J9" t="n">
-        <v>2.505610958005502</v>
+        <v>1.796853430450262</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.4940008719385482</v>
+        <v>0.3246099711920267</v>
       </c>
       <c r="L9" t="n">
-        <v>0.7139657018352998</v>
+        <v>1.899769611054289</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.755496216604165</v>
+        <v>0.4997498154989204</v>
       </c>
       <c r="N9" t="n">
-        <v>23.20588839264268</v>
+        <v>1.739176652679828</v>
       </c>
       <c r="O9" t="n">
-        <v>1.9509915279084</v>
+        <v>0.2346799848982524</v>
       </c>
       <c r="P9" t="n">
-        <v>12.21325074646995</v>
+        <v>44.28130112853792</v>
       </c>
       <c r="Q9" t="n">
-        <v>91.40785743568406</v>
+        <v>65.31648695408242</v>
       </c>
       <c r="R9" t="n">
-        <v>3.757140986830515</v>
+        <v>6.837026797469475</v>
       </c>
       <c r="S9" t="n">
-        <v>1.266326728482207</v>
+        <v>1.112762100722051</v>
       </c>
       <c r="T9" t="n">
-        <v>8.974496679188494</v>
+        <v>7.154580065904107</v>
       </c>
       <c r="U9" t="n">
-        <v>113.3461147239156</v>
+        <v>94.65997959232587</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1321683794965446</v>
+        <v>8.023644383152604</v>
       </c>
       <c r="W9" t="n">
-        <v>91.63184577749757</v>
+        <v>29.76137295080256</v>
       </c>
       <c r="X9" t="n">
-        <v>96.78823899007455</v>
+        <v>38.43102842856482</v>
       </c>
       <c r="Y9" t="n">
-        <v>28.34190155081107</v>
+        <v>52.59524350097665</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.07321010870954013</v>
+        <v>0.2753259045604256</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.202008175179574</v>
+        <v>0.8463866409673454</v>
       </c>
       <c r="AB9" t="n">
-        <v>5982.93361881297</v>
+        <v>4667.758314289911</v>
       </c>
       <c r="AC9" t="n">
-        <v>26995.46266707129</v>
+        <v>24501.680912466</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.5588711319591737</v>
+        <v>0.3136170115203303</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.7192002820485612</v>
+        <v>0.8532805207554692</v>
       </c>
       <c r="AF9" t="n">
-        <v>0.9125678371326398</v>
+        <v>0.06187260741006463</v>
       </c>
       <c r="AG9" t="n">
-        <v>0.7925425729783691</v>
+        <v>0.0573479857239846</v>
       </c>
       <c r="AH9" t="n">
-        <v>39.92761617475181</v>
+        <v>79.85972751315117</v>
       </c>
     </row>
     <row r="10">
@@ -1376,103 +1376,103 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>4.877558521269034</v>
+        <v>1.94558606055708</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1592585300396869</v>
+        <v>0.3523197903595449</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6873527371843839</v>
+        <v>2.117252970760093</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.4117411714282142</v>
+        <v>0.03382322481513222</v>
       </c>
       <c r="F10" t="n">
-        <v>0.319119201741175</v>
+        <v>1.73685598002026</v>
       </c>
       <c r="G10" t="n">
-        <v>0.04532945339321337</v>
+        <v>0.02434791078796028</v>
       </c>
       <c r="H10" t="n">
-        <v>1.902150305789989</v>
+        <v>0.5050635382393684</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8474511439266077</v>
+        <v>-0.006795246527497745</v>
       </c>
       <c r="J10" t="n">
-        <v>1.013413433293513</v>
+        <v>0.3266619771647356</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.2196318603013732</v>
+        <v>-0.08788682903869349</v>
       </c>
       <c r="L10" t="n">
-        <v>1.603986366494526</v>
+        <v>2.506072514034975</v>
       </c>
       <c r="M10" t="n">
-        <v>0.03724954646965473</v>
+        <v>-0.1509101124463803</v>
       </c>
       <c r="N10" t="n">
-        <v>13.5173352458994</v>
+        <v>23.23106232294233</v>
       </c>
       <c r="O10" t="n">
-        <v>0.6976949768141688</v>
+        <v>0.7706033466520656</v>
       </c>
       <c r="P10" t="n">
-        <v>34.33941431724461</v>
+        <v>36.4470109895454</v>
       </c>
       <c r="Q10" t="n">
-        <v>45.2389561732195</v>
+        <v>58.29534871549151</v>
       </c>
       <c r="R10" t="n">
-        <v>11.38333332691369</v>
+        <v>2.067656781517405</v>
       </c>
       <c r="S10" t="n">
-        <v>1.635108013593552</v>
+        <v>0.2292603268793557</v>
       </c>
       <c r="T10" t="n">
-        <v>1.559358014340865</v>
+        <v>5.671711301325466</v>
       </c>
       <c r="U10" t="n">
-        <v>67.96657574738076</v>
+        <v>47.61944219716902</v>
       </c>
       <c r="V10" t="n">
-        <v>4.057839009284788</v>
+        <v>6.42585587250626</v>
       </c>
       <c r="W10" t="n">
-        <v>49.67467500961252</v>
+        <v>15.70239854333698</v>
       </c>
       <c r="X10" t="n">
-        <v>59.51418624278683</v>
+        <v>12.18664493423877</v>
       </c>
       <c r="Y10" t="n">
-        <v>35.72840013743685</v>
+        <v>6.346224392067907</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.9633836232658147</v>
+        <v>0.9582923006014392</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.02720918240647462</v>
+        <v>0.3118895863924996</v>
       </c>
       <c r="AB10" t="n">
-        <v>2762.665250287385</v>
+        <v>9587.495318576728</v>
       </c>
       <c r="AC10" t="n">
-        <v>89842.99921429418</v>
+        <v>74767.87260408184</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.3425496522603988</v>
+        <v>0.5040768761539277</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.2147481852053007</v>
+        <v>0.4367604938994156</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.3571173738196041</v>
+        <v>0.613699804727306</v>
       </c>
       <c r="AG10" t="n">
-        <v>0.6258868776806582</v>
+        <v>0.3464434787836351</v>
       </c>
       <c r="AH10" t="n">
-        <v>28.34625961364161</v>
+        <v>70.29012026210282</v>
       </c>
     </row>
     <row r="11">
@@ -1480,103 +1480,2391 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>3.36162971283495</v>
+        <v>2.694474714197098</v>
       </c>
       <c r="C11" t="n">
-        <v>0.616569043796374</v>
+        <v>0.7157305210173943</v>
       </c>
       <c r="D11" t="n">
-        <v>2.633871435339334</v>
+        <v>1.148980247473667</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.9672433452712672</v>
+        <v>-0.03458635694667744</v>
       </c>
       <c r="F11" t="n">
-        <v>1.940542441378847</v>
+        <v>0.8430520607905376</v>
       </c>
       <c r="G11" t="n">
-        <v>0.8735243252233993</v>
+        <v>-0.7876607259338391</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3505468954074731</v>
+        <v>1.102118741490043</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.6722009514209075</v>
+        <v>0.04151485878460592</v>
       </c>
       <c r="J11" t="n">
-        <v>1.690024276952966</v>
+        <v>0.4981234169796719</v>
       </c>
       <c r="K11" t="n">
-        <v>0.9075227015512461</v>
+        <v>0.4876790285527552</v>
       </c>
       <c r="L11" t="n">
-        <v>0.5223980896883951</v>
+        <v>0.9472141997213614</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.4435570633067814</v>
+        <v>0.6653892737300726</v>
       </c>
       <c r="N11" t="n">
-        <v>0.9087683664309909</v>
+        <v>23.49108668172294</v>
       </c>
       <c r="O11" t="n">
-        <v>1.527605791710692</v>
+        <v>1.223351077786645</v>
       </c>
       <c r="P11" t="n">
-        <v>3.586581611533574</v>
+        <v>23.88627346374185</v>
       </c>
       <c r="Q11" t="n">
-        <v>31.68811109174428</v>
+        <v>60.59622259690956</v>
       </c>
       <c r="R11" t="n">
-        <v>17.85967753519861</v>
+        <v>3.633150508293285</v>
       </c>
       <c r="S11" t="n">
-        <v>0.6024184314058394</v>
+        <v>1.26993243786924</v>
       </c>
       <c r="T11" t="n">
-        <v>6.579160798674922</v>
+        <v>9.415888955053084</v>
       </c>
       <c r="U11" t="n">
-        <v>191.6802568915922</v>
+        <v>90.2656550509916</v>
       </c>
       <c r="V11" t="n">
-        <v>6.495120992208095</v>
+        <v>9.990210544566294</v>
       </c>
       <c r="W11" t="n">
-        <v>25.91300414577277</v>
+        <v>69.20525225335507</v>
       </c>
       <c r="X11" t="n">
-        <v>2.846365054163029</v>
+        <v>65.20777087895578</v>
       </c>
       <c r="Y11" t="n">
-        <v>67.07247495874627</v>
+        <v>67.75488870193183</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.7460082260783939</v>
+        <v>0.4988830205560322</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.4683429410886973</v>
+        <v>0.1762288624880741</v>
       </c>
       <c r="AB11" t="n">
-        <v>4206.118010827484</v>
+        <v>1024.323212855364</v>
       </c>
       <c r="AC11" t="n">
-        <v>93221.34995695428</v>
+        <v>64535.2099631595</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.07178965831985783</v>
+        <v>0.1088230615290951</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.3028630148448477</v>
+        <v>0.6940573820589867</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.2286191910815881</v>
+        <v>0.4476618175692548</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.3059888615058228</v>
+        <v>0.8403201936242148</v>
       </c>
       <c r="AH11" t="n">
-        <v>45.49376865531821</v>
+        <v>76.24714378497801</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>3.623450499347601</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.4950597000601472</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.542526546711197</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.3043273096051933</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.151644859325881</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.2080404160280358</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.04731293788517306</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-0.7846016226155779</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.325446795218383</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.8250177126630684</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.1616642574082846</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.00655771967359664</v>
+      </c>
+      <c r="N12" t="n">
+        <v>8.590809835511456</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1.405809270866364</v>
+      </c>
+      <c r="P12" t="n">
+        <v>6.263481747389791</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>86.49842183973078</v>
+      </c>
+      <c r="R12" t="n">
+        <v>14.48572698170208</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.7871020055188991</v>
+      </c>
+      <c r="T12" t="n">
+        <v>4.844929490097736</v>
+      </c>
+      <c r="U12" t="n">
+        <v>12.83775370520384</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.722417626233139</v>
+      </c>
+      <c r="W12" t="n">
+        <v>27.61055718984248</v>
+      </c>
+      <c r="X12" t="n">
+        <v>48.71658068374943</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>36.08687478849954</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.8989250524753697</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.0320870024002936</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>6070.652650528235</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>8136.353188327574</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.7633028863823652</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.9747263529624871</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.6743363983648134</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>0.4212043020086681</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>60.23406777612303</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>4.77194256259598</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8120151043134683</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.29017728691685</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.1207385482962425</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.844196793418701</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-0.1608817630266379</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.629419227645173</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-0.3080580964460962</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.040895581959457</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.6076359029818077</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.5824523006005129</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.7389292897928337</v>
+      </c>
+      <c r="N13" t="n">
+        <v>27.02566173423532</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.5943870018973296</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.3775303569263809</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>69.71615020695006</v>
+      </c>
+      <c r="R13" t="n">
+        <v>10.09525787035144</v>
+      </c>
+      <c r="S13" t="n">
+        <v>1.744612063340955</v>
+      </c>
+      <c r="T13" t="n">
+        <v>4.238284415136214</v>
+      </c>
+      <c r="U13" t="n">
+        <v>24.48059323951076</v>
+      </c>
+      <c r="V13" t="n">
+        <v>1.594631117949922</v>
+      </c>
+      <c r="W13" t="n">
+        <v>36.69519132826548</v>
+      </c>
+      <c r="X13" t="n">
+        <v>29.06157926963953</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>55.9152174647488</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.7265214331628537</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.5858024153233711</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>836.6680915157101</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>42089.4212357354</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.1932827207186161</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.3643481207117579</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0.7123718652299685</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0.512633848423403</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>32.50187742743952</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1.446337390773442</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.2876614655858274</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.421746558434648</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.2459330536511828</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.6343789461254147</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-0.6317440962340757</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.6424205894832</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.6437903235357145</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.671590000579253</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-0.00583082210935848</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2.25250059203781</v>
+      </c>
+      <c r="M14" t="n">
+        <v>-0.067009025515264</v>
+      </c>
+      <c r="N14" t="n">
+        <v>4.03255698047277</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.2755184800156888</v>
+      </c>
+      <c r="P14" t="n">
+        <v>42.93151249121562</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>20.55345547397339</v>
+      </c>
+      <c r="R14" t="n">
+        <v>4.295562322437459</v>
+      </c>
+      <c r="S14" t="n">
+        <v>1.540080103659696</v>
+      </c>
+      <c r="T14" t="n">
+        <v>8.886319294289537</v>
+      </c>
+      <c r="U14" t="n">
+        <v>3.14455714835507</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.5175923852268169</v>
+      </c>
+      <c r="W14" t="n">
+        <v>23.57719406380595</v>
+      </c>
+      <c r="X14" t="n">
+        <v>84.10470648882259</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>62.44499778200326</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.1392332913758979</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0.2776344441996069</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>7315.258720628791</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>33739.64634466577</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.7371542259819177</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.5993337064292844</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0.3055859429258346</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>0.185802437444775</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>65.58775300504227</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5.81259203312425</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.231995416338345</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.162274940347054</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.5985310651713897</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.6873717673586459</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-0.2536447893014462</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.1768598087725348</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.9046306718937933</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1.482706927018764</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.143209041168773</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.4398270598293725</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.07767272820064175</v>
+      </c>
+      <c r="N15" t="n">
+        <v>10.94337529614366</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1.32808271671475</v>
+      </c>
+      <c r="P15" t="n">
+        <v>38.75993788308559</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>26.25519918054135</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1.403497954322277</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1.151384654419764</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1.406368591055316</v>
+      </c>
+      <c r="U15" t="n">
+        <v>27.90604386218369</v>
+      </c>
+      <c r="V15" t="n">
+        <v>2.769586277840173</v>
+      </c>
+      <c r="W15" t="n">
+        <v>21.61180086668161</v>
+      </c>
+      <c r="X15" t="n">
+        <v>34.30414142053364</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>25.24300052644745</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0.3482682245667</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0.6639696010188143</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>3714.761873219048</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>97450.13669663324</v>
+      </c>
+      <c r="AD15" t="n">
+        <v>0.7949927942108157</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>0.05466640489478593</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>0.7469794354611287</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>0.9096842258708722</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>52.64184803902723</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2.115391262234895</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.3305529433757619</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.033485913921627</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.813367263765405</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.956148047166072</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-0.5727995954358939</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.188875180277501</v>
+      </c>
+      <c r="I16" t="n">
+        <v>-0.09528958100974305</v>
+      </c>
+      <c r="J16" t="n">
+        <v>2.362196877538474</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.283331824445501</v>
+      </c>
+      <c r="L16" t="n">
+        <v>2.423918100115728</v>
+      </c>
+      <c r="M16" t="n">
+        <v>-0.6682075362687445</v>
+      </c>
+      <c r="N16" t="n">
+        <v>15.45281964916697</v>
+      </c>
+      <c r="O16" t="n">
+        <v>1.71338672005329</v>
+      </c>
+      <c r="P16" t="n">
+        <v>49.25207998817658</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>52.33467305290445</v>
+      </c>
+      <c r="R16" t="n">
+        <v>11.63801696256327</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.1622168980923008</v>
+      </c>
+      <c r="T16" t="n">
+        <v>7.727910096682021</v>
+      </c>
+      <c r="U16" t="n">
+        <v>139.6790027819485</v>
+      </c>
+      <c r="V16" t="n">
+        <v>4.336789572521381</v>
+      </c>
+      <c r="W16" t="n">
+        <v>83.00468807015064</v>
+      </c>
+      <c r="X16" t="n">
+        <v>80.41454814123588</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>58.37245745283865</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.6633261414478072</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0.76360360656438</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>7015.860479660781</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>6928.851173027711</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.4987679423392066</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0.2359276107547225</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>0.8128375276210091</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>0.9527901944147136</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>45.01684061921184</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>4.613116018263529</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.6104225423941059</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.109866074254682</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.5638983794171486</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2.052730654678975</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-0.4205984762351379</v>
+      </c>
+      <c r="H17" t="n">
+        <v>2.709567683358549</v>
+      </c>
+      <c r="I17" t="n">
+        <v>-0.9112332929628745</v>
+      </c>
+      <c r="J17" t="n">
+        <v>2.621158464688565</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.4196703367891983</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1.323150669880108</v>
+      </c>
+      <c r="M17" t="n">
+        <v>-0.473846599962513</v>
+      </c>
+      <c r="N17" t="n">
+        <v>14.95487555398941</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.8492472462158485</v>
+      </c>
+      <c r="P17" t="n">
+        <v>32.2695182823537</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>79.91367403752561</v>
+      </c>
+      <c r="R17" t="n">
+        <v>9.949799574941959</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.4069006750089017</v>
+      </c>
+      <c r="T17" t="n">
+        <v>9.974835865383735</v>
+      </c>
+      <c r="U17" t="n">
+        <v>191.1247645685569</v>
+      </c>
+      <c r="V17" t="n">
+        <v>7.229908977213908</v>
+      </c>
+      <c r="W17" t="n">
+        <v>80.29017390044146</v>
+      </c>
+      <c r="X17" t="n">
+        <v>87.44884902031934</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>39.80961311317566</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.6522716738579363</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0.6460787401537292</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>9726.506851081615</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>21471.74026372697</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>0.03566732605740054</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0.5497172391783877</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>0.3680345865995479</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>0.1459928117503794</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>19.23145798364346</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>5.094289331250314</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.6835532547867171</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.391059972542306</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.5269039012563017</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2.267866119543644</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.4424851730539572</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.4023501234308464</v>
+      </c>
+      <c r="I18" t="n">
+        <v>-0.6795316765595021</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.9192296655315721</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-0.4146897954456896</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.8158691021313247</v>
+      </c>
+      <c r="M18" t="n">
+        <v>-0.5830405308406759</v>
+      </c>
+      <c r="N18" t="n">
+        <v>12.1192403037167</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1.976181285717775</v>
+      </c>
+      <c r="P18" t="n">
+        <v>9.06503024297381</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>18.31583511529907</v>
+      </c>
+      <c r="R18" t="n">
+        <v>19.86000122006296</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1.842826079124547</v>
+      </c>
+      <c r="T18" t="n">
+        <v>9.253261302776304</v>
+      </c>
+      <c r="U18" t="n">
+        <v>73.83075929568349</v>
+      </c>
+      <c r="V18" t="n">
+        <v>7.054968260519125</v>
+      </c>
+      <c r="W18" t="n">
+        <v>50.49236145265542</v>
+      </c>
+      <c r="X18" t="n">
+        <v>71.21814399898271</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>33.52047674019475</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.4462292830567509</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0.1231603602268405</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>7849.238790117402</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>14667.41614895573</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>0.6744281045385463</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>0.583263126584796</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>0.5141148782196424</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>0.7107395649620623</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>3.832064442059448</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1.63866633338441</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.2055615905871195</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.669682882314817</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-0.3497647621668122</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.01570018634059208</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.913087264898818</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2.426666759393759</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.1411082891226696</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.7152733797914546</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.2197805893642164</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.7194296336712677</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-0.3961813272499615</v>
+      </c>
+      <c r="N19" t="n">
+        <v>26.21545424443948</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.4925274235006874</v>
+      </c>
+      <c r="P19" t="n">
+        <v>22.50722345884929</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>65.95281632842664</v>
+      </c>
+      <c r="R19" t="n">
+        <v>18.82148787500518</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.2937355388775431</v>
+      </c>
+      <c r="T19" t="n">
+        <v>5.532597811026909</v>
+      </c>
+      <c r="U19" t="n">
+        <v>148.8867754239341</v>
+      </c>
+      <c r="V19" t="n">
+        <v>3.609216026550601</v>
+      </c>
+      <c r="W19" t="n">
+        <v>67.4217520928316</v>
+      </c>
+      <c r="X19" t="n">
+        <v>95.97849235276968</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>93.53543609335327</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0.7961573967822274</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>0.542780435570316</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>147.1882477279028</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>31252.50861674543</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>0.708368447198983</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0.1927494766925879</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>0.5725697238575895</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>0.2072916363611668</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>12.34997881526804</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5.4169935982043</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.8237312849253883</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.1919553492000679</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.471318230779485</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.167505109801549</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.4117317691824374</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.8660463228180723</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2051221234813481</v>
+      </c>
+      <c r="J20" t="n">
+        <v>1.20000033787242</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-0.309642002996937</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1.434898800855836</v>
+      </c>
+      <c r="M20" t="n">
+        <v>-0.2372033071695856</v>
+      </c>
+      <c r="N20" t="n">
+        <v>21.90651255547074</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.3210884180737283</v>
+      </c>
+      <c r="P20" t="n">
+        <v>19.2038727004782</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>42.56194096930076</v>
+      </c>
+      <c r="R20" t="n">
+        <v>18.3566579805752</v>
+      </c>
+      <c r="S20" t="n">
+        <v>1.228647410636115</v>
+      </c>
+      <c r="T20" t="n">
+        <v>2.476254371237042</v>
+      </c>
+      <c r="U20" t="n">
+        <v>103.6892805889516</v>
+      </c>
+      <c r="V20" t="n">
+        <v>2.378802291817869</v>
+      </c>
+      <c r="W20" t="n">
+        <v>44.8812792765473</v>
+      </c>
+      <c r="X20" t="n">
+        <v>74.78141741633276</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>93.93498066607398</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.6089594785520093</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0.9574629460730566</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>9332.864537170564</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>80874.52776152929</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.3596756629693063</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0.376653658442422</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>0.6509568269825309</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>0.4798634022865912</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>30.80410601491794</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1.4860697626595</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.6457032195307375</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.03149012121915581</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.06773731948624584</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2.624775937032805</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.29600709249247</v>
+      </c>
+      <c r="H21" t="n">
+        <v>2.100104079871843</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.2593839919635264</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1.512072757465636</v>
+      </c>
+      <c r="K21" t="n">
+        <v>-0.9963924989931896</v>
+      </c>
+      <c r="L21" t="n">
+        <v>2.965024356768103</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.1820726279788767</v>
+      </c>
+      <c r="N21" t="n">
+        <v>29.16626743833689</v>
+      </c>
+      <c r="O21" t="n">
+        <v>1.088972234136521</v>
+      </c>
+      <c r="P21" t="n">
+        <v>39.0899353730446</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>75.30948798980685</v>
+      </c>
+      <c r="R21" t="n">
+        <v>7.830152757998439</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.9318091139170797</v>
+      </c>
+      <c r="T21" t="n">
+        <v>2.986214645552176</v>
+      </c>
+      <c r="U21" t="n">
+        <v>179.4733429594582</v>
+      </c>
+      <c r="V21" t="n">
+        <v>3.402240788504536</v>
+      </c>
+      <c r="W21" t="n">
+        <v>77.02571260171192</v>
+      </c>
+      <c r="X21" t="n">
+        <v>4.607483199422107</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>20.88160789460234</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.1241156155335385</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0.8217133238230376</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>6824.312906737545</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>37927.34893612619</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0.6218657374420901</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0.007255500777292367</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0.4753448814146539</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>0.7555393396467186</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>96.960307064453</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2.31155621697647</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.2743509628678883</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.7780747891039597</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.6252133987900119</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1.574573738929075</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-0.3313603656054618</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2.041626251041666</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-0.1796881377197893</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2.461946482175925</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-0.6368507415642906</v>
+      </c>
+      <c r="L22" t="n">
+        <v>2.700329391000393</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-0.7096101524367699</v>
+      </c>
+      <c r="N22" t="n">
+        <v>20.25307973969707</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.8792551577321455</v>
+      </c>
+      <c r="P22" t="n">
+        <v>25.34068310536368</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>92.66984276887294</v>
+      </c>
+      <c r="R22" t="n">
+        <v>9.30350688142361</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.6988288460332255</v>
+      </c>
+      <c r="T22" t="n">
+        <v>5.980014365653452</v>
+      </c>
+      <c r="U22" t="n">
+        <v>165.0060329848327</v>
+      </c>
+      <c r="V22" t="n">
+        <v>5.879932424350828</v>
+      </c>
+      <c r="W22" t="n">
+        <v>41.54574557032231</v>
+      </c>
+      <c r="X22" t="n">
+        <v>66.1100957079875</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>46.96839668765661</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0.3360967658583741</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>0.9791905661269423</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>2344.700951009484</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>60538.74806883457</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>0.9985594004031154</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>0.9135180251049171</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>0.3429581111482958</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>0.7427220577225059</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>15.46525150287632</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>3.980579352061105</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.1106826332647822</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.274804779106554</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.9989307473750897</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.2554411750779008</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.7987032749739644</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2.261454714967423</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.3714480434940215</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.2422190377778197</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-0.1905170070117534</v>
+      </c>
+      <c r="L23" t="n">
+        <v>2.194950847611334</v>
+      </c>
+      <c r="M23" t="n">
+        <v>-0.9412950202088617</v>
+      </c>
+      <c r="N23" t="n">
+        <v>2.035593810706488</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.1083083218845707</v>
+      </c>
+      <c r="P23" t="n">
+        <v>41.56391053808763</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>1.787045492286946</v>
+      </c>
+      <c r="R23" t="n">
+        <v>3.032929953784729</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0.3415919021842922</v>
+      </c>
+      <c r="T23" t="n">
+        <v>3.501731396949914</v>
+      </c>
+      <c r="U23" t="n">
+        <v>80.63496266445233</v>
+      </c>
+      <c r="V23" t="n">
+        <v>9.270490474580708</v>
+      </c>
+      <c r="W23" t="n">
+        <v>12.61349524338289</v>
+      </c>
+      <c r="X23" t="n">
+        <v>57.23547980243811</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>88.81333294468399</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0.6905225330748386</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>0.08033697706943527</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>4880.673292201092</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>19380.1462728605</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>0.834784389284459</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>0.6342037805553327</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>0.257559125493512</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>0.8443645943846281</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>48.88714387847211</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2.866384263821983</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.9974740522194928</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2.528931304895994</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-0.7024891707070242</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1.025875102756194</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-0.912621984710675</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.9422033410321684</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-0.6185712064334699</v>
+      </c>
+      <c r="J24" t="n">
+        <v>2.00454081453525</v>
+      </c>
+      <c r="K24" t="n">
+        <v>-0.4498130178697817</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1.095278007995492</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.571698151810103</v>
+      </c>
+      <c r="N24" t="n">
+        <v>16.68257690233743</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1.174880942366427</v>
+      </c>
+      <c r="P24" t="n">
+        <v>13.07651326058051</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>3.632136631292659</v>
+      </c>
+      <c r="R24" t="n">
+        <v>14.34863717149926</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.1068572973358678</v>
+      </c>
+      <c r="T24" t="n">
+        <v>6.513864189050666</v>
+      </c>
+      <c r="U24" t="n">
+        <v>116.0746244356841</v>
+      </c>
+      <c r="V24" t="n">
+        <v>6.686972799406512</v>
+      </c>
+      <c r="W24" t="n">
+        <v>32.85229409556133</v>
+      </c>
+      <c r="X24" t="n">
+        <v>87.60329258872183</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>43.66936801439418</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0.5619834833105964</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>0.3324290445934664</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>5605.480107184439</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>77951.59292811961</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>0.913614989304102</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>0.1801555778531994</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>0.8112630371979651</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>0.4612292371846569</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>95.01057421431321</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>3.056321351759653</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.4546165187361925</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.751482456979236</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.7073142296174253</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2.864094578798408</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.6807681699892278</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.222187174617513</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-0.3651769555063706</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1.366687240156833</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.1192451524718914</v>
+      </c>
+      <c r="L25" t="n">
+        <v>2.847680773594111</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.9155444582185532</v>
+      </c>
+      <c r="N25" t="n">
+        <v>10.01692322536447</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.02408839160287764</v>
+      </c>
+      <c r="P25" t="n">
+        <v>27.7562630007519</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>45.12034769835716</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.6557477462493342</v>
+      </c>
+      <c r="S25" t="n">
+        <v>1.360619341966121</v>
+      </c>
+      <c r="T25" t="n">
+        <v>6.739862700678105</v>
+      </c>
+      <c r="U25" t="n">
+        <v>32.6501685623241</v>
+      </c>
+      <c r="V25" t="n">
+        <v>8.802548222056629</v>
+      </c>
+      <c r="W25" t="n">
+        <v>84.57559850634478</v>
+      </c>
+      <c r="X25" t="n">
+        <v>25.99939325240246</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>15.9121104451563</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0.3851269151781505</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>0.5286125789972563</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>3349.752935219808</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>59433.84110993145</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>0.8846268479228941</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>0.7257919120286409</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>0.2285237632709947</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>0.3164871284860183</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>81.27040274734286</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>3.934697880381792</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.5906962238323331</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.473295046686844</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.3312193690425949</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2.370699262884762</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.8588199603587243</v>
+      </c>
+      <c r="H26" t="n">
+        <v>2.937615640908716</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.7364296890755471</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2.847066090266658</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.7061627708524374</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.8878424912756205</v>
+      </c>
+      <c r="M26" t="n">
+        <v>-0.7793370298656398</v>
+      </c>
+      <c r="N26" t="n">
+        <v>14.04052373471005</v>
+      </c>
+      <c r="O26" t="n">
+        <v>1.841201277313253</v>
+      </c>
+      <c r="P26" t="n">
+        <v>15.51134185883136</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>40.1847330431543</v>
+      </c>
+      <c r="R26" t="n">
+        <v>5.129815667535152</v>
+      </c>
+      <c r="S26" t="n">
+        <v>1.786456907761136</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1.086312179241529</v>
+      </c>
+      <c r="U26" t="n">
+        <v>68.63606337675392</v>
+      </c>
+      <c r="V26" t="n">
+        <v>1.051671230793929</v>
+      </c>
+      <c r="W26" t="n">
+        <v>40.02753832181327</v>
+      </c>
+      <c r="X26" t="n">
+        <v>53.79387787387765</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>9.767373983916238</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0.5720343650753662</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>0.4192055152181786</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>4009.350744057601</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>54262.59680842023</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>0.2722827328208565</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>0.4408294734529513</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>0.4045539655597663</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>0.08047963220150947</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>16.62853648161426</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>4.203365136645258</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.9415992690652415</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.8956487667294906</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.767753207747542</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2.778195938717574</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-0.5233274058173748</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.7118047224954664</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.7943100901030657</v>
+      </c>
+      <c r="J27" t="n">
+        <v>2.223724883701539</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-0.3637739743352583</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1.799046186669709</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.2464582732767315</v>
+      </c>
+      <c r="N27" t="n">
+        <v>17.08688770113756</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1.512420209462926</v>
+      </c>
+      <c r="P27" t="n">
+        <v>28.26962371373699</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>89.02799420708364</v>
+      </c>
+      <c r="R27" t="n">
+        <v>15.70006180354567</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.9867049163718955</v>
+      </c>
+      <c r="T27" t="n">
+        <v>0.1919189983544248</v>
+      </c>
+      <c r="U27" t="n">
+        <v>57.59959480753268</v>
+      </c>
+      <c r="V27" t="n">
+        <v>2.905285547032191</v>
+      </c>
+      <c r="W27" t="n">
+        <v>97.82377331937214</v>
+      </c>
+      <c r="X27" t="n">
+        <v>76.67261071076763</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>97.38314377741746</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0.02487975945315209</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>0.3934663904827653</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>1972.584041061824</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>92576.61290055687</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>0.8669603316133689</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>0.2693367722749275</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>0.4368369672526932</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>0.6058646548085862</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>25.77109397662444</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1.1955656114434</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.8886179645024073</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2.756532838440839</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-0.9325099239101876</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.3921565922096258</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-0.4926714376301974</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2.194141856358385</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.9399126053072933</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.7813938177350463</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-0.5636244082094786</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.0554065750128912</v>
+      </c>
+      <c r="M28" t="n">
+        <v>-0.342841733480173</v>
+      </c>
+      <c r="N28" t="n">
+        <v>25.23205620641026</v>
+      </c>
+      <c r="O28" t="n">
+        <v>1.305521842701187</v>
+      </c>
+      <c r="P28" t="n">
+        <v>11.17759871022725</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>31.33064469564547</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.3881305045081637</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.5599607836637592</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1.85241679031521</v>
+      </c>
+      <c r="U28" t="n">
+        <v>160.929603181936</v>
+      </c>
+      <c r="V28" t="n">
+        <v>9.386374377397239</v>
+      </c>
+      <c r="W28" t="n">
+        <v>5.384495633241126</v>
+      </c>
+      <c r="X28" t="n">
+        <v>23.29191126209473</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>45.33131099518686</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0.5081666825867337</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>0.8031106444061278</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>451.6250023038864</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>68990.96207869727</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0.5566291443224824</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>0.3336701982884752</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>0.118869150539638</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>0.6652615278882497</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>0.7287157584054568</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>4.43021289789786</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.868415853341859</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.1587923246784787</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.4727146526116026</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1.624304900567906</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.5879272841013681</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.731990862164266</v>
+      </c>
+      <c r="I29" t="n">
+        <v>-0.2200928889512541</v>
+      </c>
+      <c r="J29" t="n">
+        <v>2.967786306721846</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-0.7537301032162478</v>
+      </c>
+      <c r="L29" t="n">
+        <v>1.268820910288832</v>
+      </c>
+      <c r="M29" t="n">
+        <v>0.3097844203595124</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.5752495503037184</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1.792780644216486</v>
+      </c>
+      <c r="P29" t="n">
+        <v>20.44524213292715</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>6.637325269467029</v>
+      </c>
+      <c r="R29" t="n">
+        <v>12.05438503369049</v>
+      </c>
+      <c r="S29" t="n">
+        <v>1.897268010499</v>
+      </c>
+      <c r="T29" t="n">
+        <v>8.2020830709031</v>
+      </c>
+      <c r="U29" t="n">
+        <v>122.3232723841325</v>
+      </c>
+      <c r="V29" t="n">
+        <v>3.948392165596453</v>
+      </c>
+      <c r="W29" t="n">
+        <v>95.9166865388946</v>
+      </c>
+      <c r="X29" t="n">
+        <v>17.55527327581224</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>76.22402572940949</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0.2201319535792002</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>0.3595189745005673</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>6494.112309626945</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>88834.83318610862</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>0.961719464574004</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>0.9497573255533823</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>0.1622688922702407</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>0.6269951115690653</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>65.70504066110109</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2.455221537081005</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.1722307698197245</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2.837126450848615</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.4190869490342244</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2.130158583611304</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.1272904580779957</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.888585210531866</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.07826455332987203</v>
+      </c>
+      <c r="J30" t="n">
+        <v>2.804872911291509</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-0.5178689188605046</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2.607792828799834</v>
+      </c>
+      <c r="M30" t="n">
+        <v>-0.9254182857263213</v>
+      </c>
+      <c r="N30" t="n">
+        <v>3.262945248570294</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1.456895593201808</v>
+      </c>
+      <c r="P30" t="n">
+        <v>3.291354416710618</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>81.84789711749507</v>
+      </c>
+      <c r="R30" t="n">
+        <v>5.667590502159271</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.4997478912694575</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1.94222688786743</v>
+      </c>
+      <c r="U30" t="n">
+        <v>126.0706000837682</v>
+      </c>
+      <c r="V30" t="n">
+        <v>7.54208486327274</v>
+      </c>
+      <c r="W30" t="n">
+        <v>65.13631815099474</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0.2114115865921539</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>82.2088402236807</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0.4319739480593012</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>0.7229282644772379</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>4214.032927225723</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>3872.757901798832</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>0.3873818209942036</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>0.8133832156720443</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>0.5409516489028626</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>0.5551315177892469</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>92.60934621993886</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3.724434780593692</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.07349305202440806</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.317691242631341</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-0.4145066945056159</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.9333212155163232</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.6959418572032592</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2.818116110468627</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-0.4987955423748025</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.6158740064510501</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.9553666615674348</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1.143845260915082</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.8453541534420059</v>
+      </c>
+      <c r="N31" t="n">
+        <v>28.04531943929556</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.1350541787813575</v>
+      </c>
+      <c r="P31" t="n">
+        <v>17.99161813838964</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>15.32976522511755</v>
+      </c>
+      <c r="R31" t="n">
+        <v>12.66270599391356</v>
+      </c>
+      <c r="S31" t="n">
+        <v>1.987926506073134</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.3197099357113535</v>
+      </c>
+      <c r="U31" t="n">
+        <v>153.3552448607567</v>
+      </c>
+      <c r="V31" t="n">
+        <v>5.163242796739834</v>
+      </c>
+      <c r="W31" t="n">
+        <v>2.647485904336301</v>
+      </c>
+      <c r="X31" t="n">
+        <v>92.01652186375955</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>79.65691391161801</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0.8436715464394301</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0.2051031008772382</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>7662.650699226859</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>94772.78817751826</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0.009338489554922041</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0.5180126008849161</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>0.8565176802300846</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0.3932792051511417</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>6.325171404587596</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>5.895280648645906</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.1423034523217959</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.7469202503170788</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-0.6600961158182237</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1.494400297404821</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-0.8306392791559082</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.1909375173375824</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.4583372084224056</v>
+      </c>
+      <c r="J32" t="n">
+        <v>2.11050584487481</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-0.8272986963491396</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.713203487016064</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.9516204496338518</v>
+      </c>
+      <c r="N32" t="n">
+        <v>5.099221511465977</v>
+      </c>
+      <c r="O32" t="n">
+        <v>1.644942462089169</v>
+      </c>
+      <c r="P32" t="n">
+        <v>34.07606915433267</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>9.712267757735175</v>
+      </c>
+      <c r="R32" t="n">
+        <v>4.989131097886968</v>
+      </c>
+      <c r="S32" t="n">
+        <v>1.061251160214177</v>
+      </c>
+      <c r="T32" t="n">
+        <v>8.594127406000812</v>
+      </c>
+      <c r="U32" t="n">
+        <v>87.17558503087686</v>
+      </c>
+      <c r="V32" t="n">
+        <v>5.415110775634361</v>
+      </c>
+      <c r="W32" t="n">
+        <v>10.40985588607027</v>
+      </c>
+      <c r="X32" t="n">
+        <v>36.49541876125122</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>64.2101166668719</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0.3012434043857941</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0.2222949087156315</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>1524.455935263358</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>87283.20420174298</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0.1562671717749171</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>0.760118638948296</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>0.9666059862238234</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>0.1201217985067464</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>90.08691441915855</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>5.267001700008169</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.05720232796205883</v>
+      </c>
+      <c r="D33" t="n">
+        <v>2.986022714481076</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-0.8644741598553409</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1.113191133870833</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.3432384205271608</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1.449366112094981</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-0.7330241529816233</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.970003502964335</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.5389329545171411</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.2382679028924495</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.5528475664170931</v>
+      </c>
+      <c r="N33" t="n">
+        <v>7.715272294907956</v>
+      </c>
+      <c r="O33" t="n">
+        <v>1.05212408043635</v>
+      </c>
+      <c r="P33" t="n">
+        <v>16.42627949375482</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>73.67905111174797</v>
+      </c>
+      <c r="R33" t="n">
+        <v>16.71491014203639</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.8160145912699186</v>
+      </c>
+      <c r="T33" t="n">
+        <v>8.087487558753367</v>
+      </c>
+      <c r="U33" t="n">
+        <v>133.7441612945149</v>
+      </c>
+      <c r="V33" t="n">
+        <v>8.494920191165736</v>
+      </c>
+      <c r="W33" t="n">
+        <v>7.815903637962715</v>
+      </c>
+      <c r="X33" t="n">
+        <v>6.467152296671269</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>24.36695926535217</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0.9921150966396645</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0.9343167041981535</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>2931.230852612117</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>10905.90375987666</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0.2328501008416673</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0.6715052206309391</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0.06426600763985259</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0.8867314314567628</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>85.12339239378969</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +3915,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>6</v>

</xml_diff>